<commit_message>
fix error codes in epp-16-ns-data
</commit_message>
<xml_diff>
--- a/data/epp-16-ns-data.xlsx
+++ b/data/epp-16-ns-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A4857-5F16-BF4A-88C7-2BE5CF8241F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ECCDEC-CF1A-B040-8F4E-0344B4F07A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
+    <workbookView xWindow="3720" yWindow="1060" windowWidth="20140" windowHeight="16240" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
   <dimension ref="B2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:F6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
@@ -880,7 +880,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I13"/>
     </row>
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I14"/>
     </row>

</xml_diff>

<commit_message>
add hostModel column (closes #28)
</commit_message>
<xml_diff>
--- a/data/epp-16-ns-data.xlsx
+++ b/data/epp-16-ns-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ECCDEC-CF1A-B040-8F4E-0344B4F07A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8557FE-FB6C-E046-A704-B426575F7F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1060" windowWidth="20140" windowHeight="16240" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>errorCode</t>
   </si>
@@ -122,6 +122,21 @@
 * Empty cells do not indicate an empty string (the "{EMPTY}" value indicates that), but will be replaced with the value in the previous row when this file is converted into YAML.
 * This means that all cells in the first row MUST be populated.
 * IP addresses must be taken from the prefixes 208.77.190.192/26 and 2602:800:900e:1257::/64 and should not be reused.</t>
+  </si>
+  <si>
+    <t>hostModel</t>
+  </si>
+  <si>
+    <t>Host model (row will be skipped if the value does not match the epp.hostModel input parameter)</t>
+  </si>
+  <si>
+    <t>objects</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>{EMPTY}</t>
   </si>
 </sst>
 </file>
@@ -198,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,9 +236,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -237,7 +249,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -338,21 +385,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -372,20 +404,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:F14" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="B7:F14" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:G18" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B7:G18" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="action" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{488E70C5-1972-EA43-AC30-4B8DD806939D}" name="createIfNeeded" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="hostname" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="0"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="hostModel" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{403394B3-820D-814C-A299-6896B22C1CAA}" name="action" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{488E70C5-1972-EA43-AC30-4B8DD806939D}" name="createIfNeeded" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="hostname" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,24 +742,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="25" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
@@ -734,79 +769,87 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="2:9" ht="128" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="9" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:10" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="2:10" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>3</v>
@@ -814,104 +857,181 @@
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I13"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I14"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I13:I14">
-    <sortCondition ref="I13:I14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J13:J14">
+    <sortCondition ref="J13:J14"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:F5"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
change error code for row #1 to EPP_DOMAIN_UPDATE_SERVER_ACCEPTS_NON_EXISTENT_HOST_OBJECT
</commit_message>
<xml_diff>
--- a/data/epp-16-ns-data.xlsx
+++ b/data/epp-16-ns-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8557FE-FB6C-E046-A704-B426575F7F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1D8089-E58B-C54D-86FC-ED53642FE179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
   <si>
     <t>errorCode</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>{EMPTY}</t>
+  </si>
+  <si>
+    <t>EPP_DOMAIN_UPDATE_SERVER_ACCEPTS_NON_EXISTENT_HOST_OBJECT</t>
   </si>
 </sst>
 </file>
@@ -234,42 +237,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -302,11 +285,16 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -385,6 +373,21 @@
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -414,12 +417,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="hostModel" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{403394B3-820D-814C-A299-6896B22C1CAA}" name="action" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{488E70C5-1972-EA43-AC30-4B8DD806939D}" name="createIfNeeded" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="hostname" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="hostModel" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{403394B3-820D-814C-A299-6896B22C1CAA}" name="action" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{488E70C5-1972-EA43-AC30-4B8DD806939D}" name="createIfNeeded" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="hostname" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -745,7 +748,7 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,7 +759,7 @@
     <col min="4" max="4" width="29.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="46.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="78" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -770,38 +773,38 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="2:10" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="2:10" ht="128" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -878,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
expand epp-16-ns-data to include IP address information for internal hosts only (only used with servers that support host attributes)
</commit_message>
<xml_diff>
--- a/data/epp-16-ns-data.xlsx
+++ b/data/epp-16-ns-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1D8089-E58B-C54D-86FC-ED53642FE179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C350F04-660C-584A-AE51-31B751443761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>errorCode</t>
   </si>
@@ -141,12 +141,96 @@
   <si>
     <t>EPP_DOMAIN_UPDATE_SERVER_ACCEPTS_NON_EXISTENT_HOST_OBJECT</t>
   </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>addr</t>
+  </si>
+  <si>
+    <t>IP address (for use with internal hosts only)</t>
+  </si>
+  <si>
+    <t>IP version (for use with internal hosts only)</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>208.77.190.196</t>
+  </si>
+  <si>
+    <t>2602:800:900e:1257::4</t>
+  </si>
+  <si>
+    <t>208.77.190</t>
+  </si>
+  <si>
+    <t>a.b.c.d</t>
+  </si>
+  <si>
+    <t>256.1.1.1</t>
+  </si>
+  <si>
+    <t>1.2.3.4.5</t>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>208.77.190.197</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>2602:800:900e:1257::5</t>
+  </si>
+  <si>
+    <t>208.77.190.198</t>
+  </si>
+  <si>
+    <t>::</t>
+  </si>
+  <si>
+    <t>::1</t>
+  </si>
+  <si>
+    <t>::X</t>
+  </si>
+  <si>
+    <t>NOT::HEX::</t>
+  </si>
+  <si>
+    <t>EPP_DOMAIN_UPDATE_SERVER_ACCEPTS_INVALID_HOST_ATTRIBUTES</t>
+  </si>
+  <si>
+    <t>EPP_DOMAIN_UPDATE_SERVER_ACCEPTS_HOST_ATTRIBUTES_WITHOUT_GLUE</t>
+  </si>
+  <si>
+    <t>{"ns2.epp-16.rst." &amp; $name}</t>
+  </si>
+  <si>
+    <t>{"ns3.epp-16.rst." &amp; $name}</t>
+  </si>
+  <si>
+    <t>{"ns4.epp-16.rst." &amp; $name}</t>
+  </si>
+  <si>
+    <t>{"ns5.epp-16.rst." &amp; $name}</t>
+  </si>
+  <si>
+    <t>{"ns6.epp-16.rst." &amp; $name}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -174,6 +258,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -195,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -212,11 +302,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF156082"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF156082"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,11 +349,57 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -407,22 +554,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:G18" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B7:G18" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:I36" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B7:I36" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="hostModel" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{403394B3-820D-814C-A299-6896B22C1CAA}" name="action" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{488E70C5-1972-EA43-AC30-4B8DD806939D}" name="createIfNeeded" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="hostname" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="0"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="hostModel" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{403394B3-820D-814C-A299-6896B22C1CAA}" name="action" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{488E70C5-1972-EA43-AC30-4B8DD806939D}" name="createIfNeeded" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="hostname" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{C04E74F4-298F-0348-BC46-BA2776462A57}" name="ip" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{2D004473-8074-A84F-9BD9-44D0BB333A8C}" name="addr" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -745,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,12 +909,14 @@
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="46.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="78" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="17.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="83.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="25" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
@@ -771,8 +924,10 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="2:10" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="2:12" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
@@ -781,15 +936,19 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="2:10" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="2:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
@@ -798,15 +957,19 @@
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
@@ -820,13 +983,19 @@
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -838,13 +1007,19 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
@@ -863,8 +1038,14 @@
       <c r="G9" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -878,13 +1059,19 @@
         <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
@@ -894,14 +1081,16 @@
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
@@ -911,14 +1100,16 @@
       <c r="E12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
@@ -928,15 +1119,17 @@
       <c r="E13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
@@ -946,15 +1139,17 @@
       <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
@@ -967,74 +1162,337 @@
       <c r="E15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>8</v>
+      <c r="G21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J13:J14">
-    <sortCondition ref="J13:J14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L13:L14">
+    <sortCondition ref="L13:L14"/>
   </sortState>
   <mergeCells count="5">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
remove the first row
</commit_message>
<xml_diff>
--- a/data/epp-16-ns-data.xlsx
+++ b/data/epp-16-ns-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAE5A13-5237-E946-BC33-9C380A8BFC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE80DD81-2A5F-7C42-A545-E0A6E3A5017C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
   <si>
     <t>errorCode</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>Host model (row will be skipped if the value does not match the epp.hostModel input parameter)</t>
-  </si>
-  <si>
-    <t>objects</t>
   </si>
   <si>
     <t>attributes</t>
@@ -219,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,9 +248,6 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,16 +255,11 @@
   <dxfs count="9">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -296,11 +285,16 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -433,8 +427,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:H18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B7:H18" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:H17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B7:H17" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -448,9 +442,9 @@
     <tableColumn id="3" xr3:uid="{403394B3-820D-814C-A299-6896B22C1CAA}" name="action" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{488E70C5-1972-EA43-AC30-4B8DD806939D}" name="createIfNeeded" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="hostname" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{2FED87FB-24A3-CB4C-B948-EE3B1A7851BB}" name="ip" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2FED87FB-24A3-CB4C-B948-EE3B1A7851BB}" name="ip" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -773,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F18"/>
+      <selection activeCell="C10" sqref="C10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>5</v>
@@ -875,7 +869,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>4</v>
@@ -908,26 +902,23 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>28</v>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
@@ -940,34 +931,34 @@
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>28</v>
+      <c r="F11" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>28</v>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
@@ -980,79 +971,79 @@
       <c r="E13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>28</v>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="K14"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>28</v>
+      <c r="F16" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.2">
@@ -1060,38 +1051,18 @@
         <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>28</v>
+      <c r="F17" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add rows for host attributes to try to add an internal host name with and without glue
</commit_message>
<xml_diff>
--- a/data/epp-16-ns-data.xlsx
+++ b/data/epp-16-ns-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE80DD81-2A5F-7C42-A545-E0A6E3A5017C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C75ABF-7239-1A4D-BF9B-63DAE93071E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
   <si>
     <t>errorCode</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>IP address to add (if any)</t>
+  </si>
+  <si>
+    <t>{"ns2.epp-16.rst." &amp; $DOMAIN}</t>
+  </si>
+  <si>
+    <t>208.77.190.200</t>
   </si>
 </sst>
 </file>
@@ -427,8 +433,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:H17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B7:H17" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:H19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B7:H19" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -767,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:K17"/>
+  <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:H10"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,6 +1072,46 @@
         <v>8</v>
       </c>
     </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K13:K14">
     <sortCondition ref="K13:K14"/>

</xml_diff>